<commit_message>
Update cloc section and continue Kotlin conversion part
</commit_message>
<xml_diff>
--- a/thesis/raw_data/cloc.xlsx
+++ b/thesis/raw_data/cloc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daviddrews/Development/lens-david/thesis/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3AFD9B-C4CC-E747-8CA4-FF0CBF0575F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3228D538-57F0-C84C-8DE7-276B9C15A5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20460" activeTab="1" xr2:uid="{A3A511C6-B65E-4047-BA88-427099B7032B}"/>
+    <workbookView xWindow="51200" yWindow="12500" windowWidth="30720" windowHeight="18700" activeTab="1" xr2:uid="{A3A511C6-B65E-4047-BA88-427099B7032B}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="103">
   <si>
     <t>File</t>
   </si>
@@ -304,10 +304,49 @@
     <t>ViewFinder</t>
   </si>
   <si>
-    <t>Code Delta</t>
-  </si>
-  <si>
-    <t>SUM</t>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>\begin{table}[H]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		\hline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	\begin{tabularx}{\columnwidth}</t>
+  </si>
+  <si>
+    <t>\end{table}</t>
+  </si>
+  <si>
+    <t>\\</t>
+  </si>
+  <si>
+    <t>\hline \hline</t>
+  </si>
+  <si>
+    <t>\hline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	\end{tabularx}</t>
+  </si>
+  <si>
+    <t>\label{tab:cloc}</t>
+  </si>
+  <si>
+    <t>\bfseries{Cumulative Delta Over All Java Files}</t>
+  </si>
+  <si>
+    <t>{ &gt;{\RaggedRight}p{9cm} | C }</t>
+  </si>
+  <si>
+    <t>\caption[Java Files in TUM-Lens v1.0 And Change in Lines of Code After Their Conversion to Kotlin]{This table shows the results from the command line prompt in listing \ref{code:cloc}. Packages have been indicated as a prefix to the file name to resemble the original project structure of TUM-Lens v1.0. Overall, the total size of the codebase shrank because of the migration from Java to Kotlin. This is particularly impressive as understandably further logic needed to be added to existing classes in order to account for the new object detection functionality.}</t>
+  </si>
+  <si>
+    <t>Files migrated from Java to Kotlin (extension omitted)</t>
+  </si>
+  <si>
+    <t>Delta in lines of code</t>
   </si>
 </sst>
 </file>
@@ -351,9 +390,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3051,251 +3093,525 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DDAEDA-F566-CF49-8087-CF5BD3DE5946}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="B2:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>64</v>
       </c>
-      <c r="B2">
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7">
         <f>-data!O2+data!N3</f>
         <v>-34</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>65</v>
       </c>
-      <c r="B3">
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8">
         <f>-data!O4+data!N5</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9">
+        <f>-data!O42+data!N43</f>
+        <v>-9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10">
+        <f>-data!O44+data!N45</f>
+        <v>-8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11">
+        <f>-data!O46+data!N47</f>
+        <v>-12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12">
+        <f>-data!O48+data!N49</f>
+        <v>-7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>66</v>
       </c>
-      <c r="B4">
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13">
         <f>-data!O6+data!N7</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>67</v>
       </c>
-      <c r="B5">
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14">
         <f>-data!O8+data!N9</f>
         <v>-15</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>68</v>
       </c>
-      <c r="B6">
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15">
         <f>-data!O10+data!N11</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>69</v>
       </c>
-      <c r="B7">
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16">
         <f>-data!O12+data!N13</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="E16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>70</v>
       </c>
-      <c r="B8">
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17">
         <f>-data!O14+data!N15</f>
         <v>-7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>71</v>
       </c>
-      <c r="B9">
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18">
         <f>-data!O16+data!N17</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="E18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="B10">
+      <c r="C19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19">
         <f>-data!O18+data!N19</f>
         <v>-6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>73</v>
       </c>
-      <c r="B11">
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20">
         <f>-data!O20+data!N21</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>74</v>
       </c>
-      <c r="B12">
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21">
         <f>-data!O22+data!N23</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>75</v>
       </c>
-      <c r="B13">
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22">
         <f>-data!O24+data!N25</f>
         <v>-6</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>76</v>
       </c>
-      <c r="B14">
+      <c r="C23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23">
         <f>-data!O26+data!N27</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="E23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>77</v>
       </c>
-      <c r="B15">
+      <c r="C24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24">
         <f>-data!O28+data!N29</f>
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="E24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>78</v>
       </c>
-      <c r="B16">
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25">
         <f>-data!O30+data!N31</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>79</v>
       </c>
-      <c r="B17">
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26">
         <f>-data!O32+data!N33</f>
         <v>-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="E26" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>80</v>
       </c>
-      <c r="B18">
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27">
         <f>-data!O34+data!N35</f>
         <v>-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>81</v>
       </c>
-      <c r="B19">
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28">
         <f>-data!O36+data!N37</f>
         <v>-26</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="E28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>82</v>
       </c>
-      <c r="B20">
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29">
         <f>-data!O38+data!N39</f>
         <v>-21</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="E29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>83</v>
       </c>
-      <c r="B21">
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30">
         <f>-data!O40+data!N41</f>
         <v>-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22">
-        <f>-data!O42+data!N43</f>
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23">
-        <f>-data!O44+data!N45</f>
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24">
-        <f>-data!O46+data!N47</f>
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25">
-        <f>-data!O48+data!N49</f>
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="1">
-        <f>SUM(B2:B26)</f>
-        <v>-79</v>
+      <c r="E30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="1" t="str">
+        <f>"\bfseries{"&amp;SUM(D7:D30)&amp;"}"</f>
+        <v>\bfseries{-79}</v>
+      </c>
+      <c r="E31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>